<commit_message>
#2 Files are attempt to test splitting the system into PQ and PV buses
base case doesn't converge on a solution within 50 iterations. Creating a new workspace to test a different way of solving bus data.
</commit_message>
<xml_diff>
--- a/system_basecase.xlsx
+++ b/system_basecase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baumj\Documents\UW Courses\EE 454 - Power System Analysis\Fall 2018\454project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Documents\UW\A19\EE 454\Project\EE454\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF0C301-A935-4F31-BDEA-4FC440D27BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC963A8B-28FF-418B-8538-7DBE38354B26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2532" yWindow="2532" windowWidth="9900" windowHeight="9738" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BusData" sheetId="1" r:id="rId1"/>
@@ -396,13 +396,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -442,7 +442,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -462,7 +462,7 @@
         <v>1.0449999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
@@ -482,7 +482,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
@@ -502,7 +502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
@@ -542,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
@@ -582,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
@@ -622,7 +622,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
@@ -642,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
@@ -672,13 +672,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -698,7 +698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -718,7 +718,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
@@ -738,7 +738,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2</v>
       </c>
@@ -758,7 +758,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>2</v>
       </c>
@@ -778,7 +778,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>2</v>
       </c>
@@ -798,7 +798,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>3</v>
       </c>
@@ -818,7 +818,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>4</v>
       </c>
@@ -838,7 +838,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>4</v>
       </c>
@@ -858,7 +858,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>5</v>
       </c>
@@ -878,7 +878,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>6</v>
       </c>
@@ -898,7 +898,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>6</v>
       </c>
@@ -918,7 +918,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>6</v>
       </c>
@@ -938,7 +938,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>7</v>
       </c>
@@ -958,7 +958,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>7</v>
       </c>
@@ -978,7 +978,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>8</v>
       </c>
@@ -998,7 +998,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Contingency case 1 and 2 added
</commit_message>
<xml_diff>
--- a/system_basecase.xlsx
+++ b/system_basecase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Documents\UW\A19\EE 454\Project\EE454\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eliot Nichols\Documents\GitHub\EE454\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AF21B8-D34E-4EFE-8D75-6B7AC673B2AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1DC904-FF99-4B76-B05D-092B600433C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BusData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="ContingencyCase1" sheetId="3" r:id="rId3"/>
     <sheet name="ContingencyCase2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -399,12 +401,12 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -444,7 +446,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -464,7 +466,7 @@
         <v>1.0449999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -484,7 +486,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -504,7 +506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -524,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -544,7 +546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -564,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -584,7 +586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -604,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -624,7 +626,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -644,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -675,12 +677,12 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="A1:F18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -700,7 +702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -720,7 +722,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -740,7 +742,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -760,7 +762,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -780,7 +782,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -800,7 +802,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -820,7 +822,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -840,7 +842,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -860,7 +862,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -880,7 +882,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -900,7 +902,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -920,7 +922,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -940,7 +942,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -960,7 +962,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -980,7 +982,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1000,7 +1002,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1020,7 +1022,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1047,15 +1049,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4A2F40-2156-471F-99B6-581E07FCDA91}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1075,7 +1077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1099,7 +1101,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1119,7 +1121,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1139,7 +1141,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1159,7 +1161,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1179,7 +1181,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1199,7 +1201,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1219,7 +1221,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1239,7 +1241,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1259,7 +1261,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -1279,7 +1281,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1299,7 +1301,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1339,7 +1341,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1359,7 +1361,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1379,23 +1381,43 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
         <v>11</v>
       </c>
-      <c r="B17">
+      <c r="C17">
+        <v>0.22092000000000001</v>
+      </c>
+      <c r="D17">
+        <v>0.19988</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
         <v>12</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>0.17093</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>0.34802</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
         <v>9999</v>
       </c>
     </row>
@@ -1406,15 +1428,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0752CE19-70B3-4BB8-8F64-4BA81CD30F7F}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1434,7 +1456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1454,7 +1476,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1474,7 +1496,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1494,7 +1516,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1514,7 +1536,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1534,7 +1556,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1554,7 +1576,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1574,7 +1596,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1594,7 +1616,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1614,7 +1636,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -1634,7 +1656,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1654,7 +1676,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1674,7 +1696,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1694,7 +1716,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1714,7 +1736,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1734,43 +1756,23 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <v>0.22092000000000001</v>
+        <v>0.17093</v>
       </c>
       <c r="D17">
-        <v>0.19988</v>
+        <v>0.34802</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
-        <v>11</v>
-      </c>
-      <c r="B18">
-        <v>12</v>
-      </c>
-      <c r="C18">
-        <v>0.17093</v>
-      </c>
-      <c r="D18">
-        <v>0.34802</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
         <v>9999</v>
       </c>
     </row>

</xml_diff>